<commit_message>
cambios menores en algunos ficheros. Programa probado en nave 1
</commit_message>
<xml_diff>
--- a/VARIOS/2023_8472_GloriaGea_NAVE1_ADSORCION.xlsx
+++ b/VARIOS/2023_8472_GloriaGea_NAVE1_ADSORCION.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unizares-my.sharepoint.com/personal/ptellez_unizar_es/Documents/INSTRUMENTACION/TRABAJOS_2023/__2023_8472_GloriaGea_NAVE1up_ADSORCION/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\OneDrive - unizar.es\INSTRUMENTACION\TRABAJOS_2023\__2023_8472_GloriaGea_NAVE1up_ADSORCION\VARIOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="86">
   <si>
     <t>FARNELL</t>
   </si>
@@ -222,30 +222,15 @@
     <t>MATERIAL</t>
   </si>
   <si>
-    <t>PLASTICO TAPA TRASPARENTE S.70 145x90x45</t>
-  </si>
-  <si>
     <t>CONVERTIDOR</t>
   </si>
   <si>
     <t>FTDI Chip USB-COM485-Plus1</t>
   </si>
   <si>
-    <t>F 62717913</t>
-  </si>
-  <si>
-    <t>A 16252222</t>
-  </si>
-  <si>
     <t>CABLE USB</t>
   </si>
   <si>
-    <t>C48010</t>
-  </si>
-  <si>
-    <t>CABLE USB-A USB-B</t>
-  </si>
-  <si>
     <t>PLANTA ADSORCION</t>
   </si>
   <si>
@@ -255,9 +240,6 @@
     <t>HUB USB</t>
   </si>
   <si>
-    <t>HUB USB 4xPORT A</t>
-  </si>
-  <si>
     <t>RELE</t>
   </si>
   <si>
@@ -270,9 +252,6 @@
     <t>TARJETA RELEx1 M5STACK</t>
   </si>
   <si>
-    <t>CABLE USB-A USB-C</t>
-  </si>
-  <si>
     <t>CAJA RELE</t>
   </si>
   <si>
@@ -280,6 +259,33 @@
   </si>
   <si>
     <t>USB USB</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> HUB 4 X USB 2.0</t>
+  </si>
+  <si>
+    <t>F4205709</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 38.452/2</t>
+  </si>
+  <si>
+    <t>CABLE USB-A USB-C 38.452/2  2M</t>
+  </si>
+  <si>
+    <t>F4204932</t>
+  </si>
+  <si>
+    <t>F62798459</t>
+  </si>
+  <si>
+    <t>F62717913</t>
+  </si>
+  <si>
+    <t>F4200619</t>
+  </si>
+  <si>
+    <t>33070211 CAJA S.70 NEGRA 145X90X45</t>
   </si>
 </sst>
 </file>
@@ -395,7 +401,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -471,6 +477,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -602,7 +614,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -732,53 +744,56 @@
     <xf numFmtId="164" fontId="3" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="12" fillId="10" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="10" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1160,8 +1175,8 @@
   </sheetPr>
   <dimension ref="A1:V43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="C7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1192,80 +1207,80 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="15" x14ac:dyDescent="0.2">
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="56"/>
+      <c r="M1" s="56"/>
+      <c r="N1" s="56"/>
+      <c r="O1" s="56"/>
     </row>
     <row r="2" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="55" t="s">
-        <v>72</v>
-      </c>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
-      <c r="J2" s="55"/>
-      <c r="K2" s="55"/>
-      <c r="L2" s="55"/>
-      <c r="M2" s="55"/>
-      <c r="N2" s="55"/>
-      <c r="O2" s="55"/>
+      <c r="B2" s="57" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="57"/>
+      <c r="K2" s="57"/>
+      <c r="L2" s="57"/>
+      <c r="M2" s="57"/>
+      <c r="N2" s="57"/>
+      <c r="O2" s="57"/>
       <c r="U2" s="5"/>
       <c r="V2" s="5"/>
     </row>
     <row r="3" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="57"/>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="57"/>
-      <c r="G3" s="57"/>
-      <c r="H3" s="57"/>
-      <c r="I3" s="57"/>
-      <c r="J3" s="57"/>
-      <c r="K3" s="57"/>
-      <c r="L3" s="57"/>
-      <c r="M3" s="57"/>
-      <c r="N3" s="57"/>
-      <c r="O3" s="57"/>
+      <c r="B3" s="60"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="60"/>
+      <c r="H3" s="60"/>
+      <c r="I3" s="60"/>
+      <c r="J3" s="60"/>
+      <c r="K3" s="60"/>
+      <c r="L3" s="60"/>
+      <c r="M3" s="60"/>
+      <c r="N3" s="60"/>
+      <c r="O3" s="60"/>
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
       <c r="S3" s="2"/>
       <c r="T3" s="2"/>
     </row>
     <row r="4" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="57" t="s">
-        <v>73</v>
-      </c>
-      <c r="C4" s="57"/>
-      <c r="D4" s="57"/>
-      <c r="E4" s="57"/>
-      <c r="F4" s="57"/>
-      <c r="G4" s="57"/>
-      <c r="H4" s="57"/>
-      <c r="I4" s="57"/>
-      <c r="J4" s="57"/>
-      <c r="K4" s="57"/>
-      <c r="L4" s="57"/>
-      <c r="M4" s="57"/>
-      <c r="N4" s="57"/>
-      <c r="O4" s="57"/>
+      <c r="B4" s="60" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="60"/>
+      <c r="H4" s="60"/>
+      <c r="I4" s="60"/>
+      <c r="J4" s="60"/>
+      <c r="K4" s="60"/>
+      <c r="L4" s="60"/>
+      <c r="M4" s="60"/>
+      <c r="N4" s="60"/>
+      <c r="O4" s="60"/>
       <c r="Q4" s="4"/>
       <c r="R4" s="4"/>
       <c r="S4" s="4"/>
@@ -1279,17 +1294,17 @@
       <c r="S5" s="4"/>
     </row>
     <row r="6" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="47" t="s">
+      <c r="B6" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="47"/>
-      <c r="D6" s="47"/>
-      <c r="E6" s="47"/>
-      <c r="F6" s="47"/>
-      <c r="G6" s="47"/>
-      <c r="H6" s="47"/>
-      <c r="I6" s="47"/>
-      <c r="J6" s="47"/>
+      <c r="C6" s="59"/>
+      <c r="D6" s="59"/>
+      <c r="E6" s="59"/>
+      <c r="F6" s="59"/>
+      <c r="G6" s="59"/>
+      <c r="H6" s="59"/>
+      <c r="I6" s="59"/>
+      <c r="J6" s="59"/>
       <c r="K6" s="26"/>
       <c r="L6" s="14" t="s">
         <v>10</v>
@@ -1334,12 +1349,12 @@
         <v>52</v>
       </c>
       <c r="K7" s="26"/>
-      <c r="L7" s="56" t="s">
+      <c r="L7" s="58" t="s">
         <v>50</v>
       </c>
-      <c r="M7" s="56"/>
-      <c r="N7" s="56"/>
-      <c r="O7" s="56"/>
+      <c r="M7" s="58"/>
+      <c r="N7" s="58"/>
+      <c r="O7" s="58"/>
       <c r="Q7" s="4"/>
       <c r="R7" s="4"/>
       <c r="S7" s="4"/>
@@ -1356,11 +1371,11 @@
       </c>
       <c r="E8" s="30">
         <f>$F$31</f>
-        <v>0</v>
+        <v>54.88000000000001</v>
       </c>
       <c r="F8" s="22">
         <f t="shared" ref="F8" si="0">D8*E8</f>
-        <v>0</v>
+        <v>54.88000000000001</v>
       </c>
       <c r="G8" s="34" t="s">
         <v>46</v>
@@ -1399,7 +1414,7 @@
         <v>27</v>
       </c>
       <c r="M9" s="12">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="N9" s="8">
         <f>Referencias!G2</f>
@@ -1407,7 +1422,7 @@
       </c>
       <c r="O9" s="8">
         <f>M9*N9</f>
-        <v>0</v>
+        <v>282</v>
       </c>
       <c r="Q9" s="4"/>
       <c r="R9" s="4"/>
@@ -1499,30 +1514,30 @@
       <c r="E13" s="31"/>
       <c r="F13" s="23">
         <f>SUBTOTAL(109,F8:F12)</f>
-        <v>0</v>
+        <v>54.88000000000001</v>
       </c>
       <c r="G13" s="35"/>
       <c r="H13" s="7"/>
       <c r="I13" s="35"/>
       <c r="J13" s="44"/>
-      <c r="L13" s="52" t="s">
+      <c r="L13" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="M13" s="52"/>
-      <c r="N13" s="58">
+      <c r="M13" s="49"/>
+      <c r="N13" s="47">
         <f>SUM(O9:O12)</f>
-        <v>71.25</v>
-      </c>
-      <c r="O13" s="58"/>
+        <v>353.25</v>
+      </c>
+      <c r="O13" s="47"/>
       <c r="Q13" s="4"/>
       <c r="R13" s="4"/>
       <c r="S13" s="4"/>
     </row>
     <row r="14" spans="1:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L14" s="53"/>
-      <c r="M14" s="53"/>
-      <c r="N14" s="59"/>
-      <c r="O14" s="59"/>
+      <c r="L14" s="50"/>
+      <c r="M14" s="50"/>
+      <c r="N14" s="48"/>
+      <c r="O14" s="48"/>
       <c r="Q14" s="4"/>
       <c r="R14" s="4"/>
       <c r="S14" s="4"/>
@@ -1533,23 +1548,23 @@
       <c r="S15" s="4"/>
     </row>
     <row r="16" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="47" t="s">
+      <c r="B16" s="59" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="47"/>
-      <c r="D16" s="47"/>
-      <c r="E16" s="47"/>
-      <c r="F16" s="47"/>
-      <c r="G16" s="47"/>
-      <c r="H16" s="47"/>
-      <c r="I16" s="47"/>
-      <c r="J16" s="47"/>
-      <c r="L16" s="60" t="s">
+      <c r="C16" s="59"/>
+      <c r="D16" s="59"/>
+      <c r="E16" s="59"/>
+      <c r="F16" s="59"/>
+      <c r="G16" s="59"/>
+      <c r="H16" s="59"/>
+      <c r="I16" s="59"/>
+      <c r="J16" s="59"/>
+      <c r="L16" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="M16" s="60"/>
-      <c r="N16" s="60"/>
-      <c r="O16" s="60"/>
+      <c r="M16" s="51"/>
+      <c r="N16" s="51"/>
+      <c r="O16" s="51"/>
       <c r="Q16" s="4"/>
       <c r="R16" s="4"/>
       <c r="S16" s="4"/>
@@ -1582,10 +1597,10 @@
       <c r="J17" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="L17" s="61" t="s">
+      <c r="L17" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="M17" s="62"/>
+      <c r="M17" s="53"/>
       <c r="N17" s="18" t="s">
         <v>43</v>
       </c>
@@ -1598,7 +1613,7 @@
     </row>
     <row r="18" spans="2:19" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B18" s="45" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C18" s="32"/>
       <c r="D18" s="37"/>
@@ -1608,14 +1623,14 @@
       <c r="H18" s="27"/>
       <c r="I18" s="34"/>
       <c r="J18" s="43"/>
-      <c r="L18" s="48" t="s">
+      <c r="L18" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="M18" s="49"/>
+      <c r="M18" s="62"/>
       <c r="N18" s="19"/>
       <c r="O18" s="19">
         <f>N13</f>
-        <v>71.25</v>
+        <v>353.25</v>
       </c>
       <c r="Q18" s="4"/>
       <c r="R18" s="4"/>
@@ -1623,31 +1638,37 @@
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B19" s="32" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C19" s="36" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D19" s="37">
         <v>1</v>
       </c>
       <c r="E19" s="30">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F19" s="22">
         <f t="shared" ref="F19" si="2">D19*E19</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G19" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="H19" s="27"/>
-      <c r="I19" s="34"/>
-      <c r="J19" s="43"/>
-      <c r="L19" s="50" t="s">
+      <c r="H19" s="27">
+        <v>151301</v>
+      </c>
+      <c r="I19" s="63" t="s">
+        <v>78</v>
+      </c>
+      <c r="J19" s="43">
+        <v>44757</v>
+      </c>
+      <c r="L19" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="M19" s="51"/>
+      <c r="M19" s="55"/>
       <c r="N19" s="19"/>
       <c r="O19" s="19"/>
       <c r="Q19" s="4"/>
@@ -1656,7 +1677,7 @@
     </row>
     <row r="20" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B20" s="45" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="C20" s="36"/>
       <c r="D20" s="37"/>
@@ -1666,17 +1687,17 @@
       <c r="H20" s="27"/>
       <c r="I20" s="34"/>
       <c r="J20" s="43"/>
-      <c r="L20" s="50" t="s">
+      <c r="L20" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="M20" s="51"/>
+      <c r="M20" s="55"/>
       <c r="N20" s="19">
         <f>F13</f>
-        <v>0</v>
+        <v>54.88000000000001</v>
       </c>
       <c r="O20" s="19">
         <f>N20</f>
-        <v>0</v>
+        <v>54.88000000000001</v>
       </c>
       <c r="Q20" s="4"/>
       <c r="R20" s="4"/>
@@ -1687,17 +1708,17 @@
         <v>61</v>
       </c>
       <c r="C21" s="36" t="s">
-        <v>64</v>
+        <v>85</v>
       </c>
       <c r="D21" s="37">
         <v>1</v>
       </c>
       <c r="E21" s="30">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F21" s="22">
         <f t="shared" ref="F21:F22" si="3">D21*E21</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G21" s="34" t="s">
         <v>41</v>
@@ -1705,16 +1726,16 @@
       <c r="H21" s="27">
         <v>33070211</v>
       </c>
-      <c r="I21" s="34" t="s">
-        <v>68</v>
+      <c r="I21" s="63" t="s">
+        <v>84</v>
       </c>
       <c r="J21" s="43">
-        <v>44552</v>
-      </c>
-      <c r="L21" s="50" t="s">
+        <v>44595</v>
+      </c>
+      <c r="L21" s="54" t="s">
         <v>45</v>
       </c>
-      <c r="M21" s="51"/>
+      <c r="M21" s="55"/>
       <c r="N21" s="19"/>
       <c r="O21" s="19"/>
       <c r="Q21" s="4"/>
@@ -1723,76 +1744,82 @@
     </row>
     <row r="22" spans="2:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="32" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C22" s="36" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="D22" s="37">
         <v>1</v>
       </c>
       <c r="E22" s="46">
-        <v>0</v>
+        <v>3.32</v>
       </c>
       <c r="F22" s="22">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3.32</v>
       </c>
       <c r="G22" s="34" t="s">
         <v>2</v>
       </c>
       <c r="H22" s="27"/>
-      <c r="I22" s="34" t="s">
-        <v>67</v>
-      </c>
-      <c r="J22" s="43"/>
-      <c r="L22" s="52" t="s">
+      <c r="I22" s="63" t="s">
+        <v>82</v>
+      </c>
+      <c r="J22" s="43">
+        <v>44753</v>
+      </c>
+      <c r="L22" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="M22" s="52"/>
-      <c r="N22" s="58">
+      <c r="M22" s="49"/>
+      <c r="N22" s="47">
         <f>SUM(O18:O21)</f>
-        <v>71.25</v>
-      </c>
-      <c r="O22" s="58"/>
+        <v>408.13</v>
+      </c>
+      <c r="O22" s="47"/>
       <c r="Q22" s="4"/>
       <c r="R22" s="4"/>
       <c r="S22" s="4"/>
     </row>
     <row r="23" spans="2:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="32" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C23" s="36" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="D23" s="37">
         <v>1</v>
       </c>
       <c r="E23" s="30">
-        <v>0</v>
+        <v>3.74</v>
       </c>
       <c r="F23" s="22">
         <f t="shared" ref="F23:F24" si="4">D23*E23</f>
-        <v>0</v>
+        <v>3.74</v>
       </c>
       <c r="G23" s="34" t="s">
         <v>2</v>
       </c>
       <c r="H23" s="27"/>
-      <c r="I23" s="34"/>
-      <c r="J23" s="43"/>
-      <c r="L23" s="53"/>
-      <c r="M23" s="53"/>
-      <c r="N23" s="59"/>
-      <c r="O23" s="59"/>
+      <c r="I23" s="63" t="s">
+        <v>83</v>
+      </c>
+      <c r="J23" s="43">
+        <v>44684</v>
+      </c>
+      <c r="L23" s="50"/>
+      <c r="M23" s="50"/>
+      <c r="N23" s="48"/>
+      <c r="O23" s="48"/>
       <c r="Q23" s="4"/>
       <c r="R23" s="4"/>
       <c r="S23" s="4"/>
     </row>
     <row r="24" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B24" s="32" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C24" s="36" t="s">
         <v>80</v>
@@ -1801,27 +1828,31 @@
         <v>1</v>
       </c>
       <c r="E24" s="30">
-        <v>0</v>
+        <v>3.2</v>
       </c>
       <c r="F24" s="22">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>3.2</v>
       </c>
       <c r="G24" s="34" t="s">
         <v>41</v>
       </c>
       <c r="H24" s="27" t="s">
-        <v>70</v>
-      </c>
-      <c r="I24" s="34"/>
-      <c r="J24" s="43"/>
+        <v>79</v>
+      </c>
+      <c r="I24" s="63" t="s">
+        <v>81</v>
+      </c>
+      <c r="J24" s="43">
+        <v>44732</v>
+      </c>
       <c r="Q24" s="4"/>
       <c r="R24" s="4"/>
       <c r="S24" s="4"/>
     </row>
     <row r="25" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B25" s="45" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C25" s="36"/>
       <c r="D25" s="37"/>
@@ -1837,20 +1868,20 @@
     </row>
     <row r="26" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B26" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="C26" s="36" t="s">
         <v>65</v>
-      </c>
-      <c r="C26" s="36" t="s">
-        <v>66</v>
       </c>
       <c r="D26" s="37">
         <v>1</v>
       </c>
       <c r="E26" s="30">
-        <v>0</v>
+        <v>31.42</v>
       </c>
       <c r="F26" s="22">
-        <f t="shared" ref="F26" si="5">D26*E26</f>
-        <v>0</v>
+        <f t="shared" ref="F26:F27" si="5">D26*E26</f>
+        <v>31.42</v>
       </c>
       <c r="G26" s="34" t="s">
         <v>2</v>
@@ -1858,11 +1889,11 @@
       <c r="H26" s="27">
         <v>6877746</v>
       </c>
-      <c r="I26" s="34" t="s">
-        <v>67</v>
+      <c r="I26" s="63" t="s">
+        <v>82</v>
       </c>
       <c r="J26" s="43">
-        <v>44684</v>
+        <v>44819</v>
       </c>
       <c r="L26" s="5"/>
       <c r="M26" s="5"/>
@@ -1873,29 +1904,33 @@
     </row>
     <row r="27" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B27" s="32" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C27" s="36" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="D27" s="37">
         <v>1</v>
       </c>
       <c r="E27" s="30">
-        <v>0</v>
+        <v>3.2</v>
       </c>
       <c r="F27" s="22">
-        <f t="shared" ref="F27" si="6">D27*E27</f>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>3.2</v>
       </c>
       <c r="G27" s="34" t="s">
         <v>41</v>
       </c>
       <c r="H27" s="27" t="s">
-        <v>70</v>
-      </c>
-      <c r="I27" s="34"/>
-      <c r="J27" s="43"/>
+        <v>79</v>
+      </c>
+      <c r="I27" s="63" t="s">
+        <v>81</v>
+      </c>
+      <c r="J27" s="43">
+        <v>44732</v>
+      </c>
       <c r="L27" s="5"/>
       <c r="M27" s="5"/>
       <c r="P27" s="4"/>
@@ -1965,7 +2000,7 @@
       <c r="E31" s="31"/>
       <c r="F31" s="23">
         <f>SUBTOTAL(109,F21:F30)*D31</f>
-        <v>0</v>
+        <v>54.88000000000001</v>
       </c>
       <c r="G31" s="35"/>
       <c r="H31" s="7"/>
@@ -2076,23 +2111,23 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="B16:J16"/>
+    <mergeCell ref="L18:M18"/>
+    <mergeCell ref="L20:M20"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="L22:M23"/>
+    <mergeCell ref="B1:O1"/>
+    <mergeCell ref="B2:O2"/>
+    <mergeCell ref="L7:O7"/>
+    <mergeCell ref="B6:J6"/>
+    <mergeCell ref="B3:O3"/>
+    <mergeCell ref="B4:O4"/>
     <mergeCell ref="N22:O23"/>
     <mergeCell ref="N13:O14"/>
     <mergeCell ref="L13:M14"/>
     <mergeCell ref="L16:O16"/>
     <mergeCell ref="L17:M17"/>
     <mergeCell ref="L19:M19"/>
-    <mergeCell ref="B1:O1"/>
-    <mergeCell ref="B2:O2"/>
-    <mergeCell ref="L7:O7"/>
-    <mergeCell ref="B6:J6"/>
-    <mergeCell ref="B3:O3"/>
-    <mergeCell ref="B4:O4"/>
-    <mergeCell ref="B16:J16"/>
-    <mergeCell ref="L18:M18"/>
-    <mergeCell ref="L20:M20"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="L22:M23"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <dataValidations count="1">
@@ -2404,15 +2439,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010049DC05B388A41B45A6040073BCA884BD" ma:contentTypeVersion="9" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="191824848219d90cb14cca2632b26800">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="78edefa9-fd3d-41c6-a7e0-7a5c8261beba" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="06d538f224d06ce15cc775e8607d670f" ns3:_="">
     <xsd:import namespace="78edefa9-fd3d-41c6-a7e0-7a5c8261beba"/>
@@ -2588,6 +2614,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2595,14 +2630,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F3B223F8-31F8-4BEB-90EC-F64E9AFAD4FC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3D754679-E9AE-4E01-9374-78E1988BE193}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2620,17 +2647,25 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F3B223F8-31F8-4BEB-90EC-F64E9AFAD4FC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE3F0589-E4E8-49E7-8E35-8C71F2C4EF9E}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="78edefa9-fd3d-41c6-a7e0-7a5c8261beba"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>

</xml_diff>